<commit_message>
ficha 5 completa, ficha 6 ex1
</commit_message>
<xml_diff>
--- a/Exercicios/out/production/Exercicios/Ficha5/ex4/ex4.xlsx
+++ b/Exercicios/out/production/Exercicios/Ficha5/ex4/ex4.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\ED_Pratica\Exercicios\src\Ficha5\ex4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEABF18-1B15-4DD3-876C-DECE989148C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2432E6-5ED8-4E34-BDF7-A2BC89AAF7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ex4" sheetId="2" r:id="rId1"/>
-    <sheet name="Folha1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="DadosExternos_1" localSheetId="0" hidden="1">'ex4'!$A$1:$C$31</definedName>
@@ -1694,7 +1693,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C31"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2051,18 +2050,6 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>